<commit_message>
Updating raw data and fetching raw data in one go
</commit_message>
<xml_diff>
--- a/data_raw/CME_BRR_latest.xlsx
+++ b/data_raw/CME_BRR_latest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D437"/>
+  <dimension ref="A1:D444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7431,6 +7431,118 @@
         <v>112643.89</v>
       </c>
     </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>2025-09-06</t>
+        </is>
+      </c>
+      <c r="B438" t="n">
+        <v>110904.6</v>
+      </c>
+      <c r="C438" t="n">
+        <v>110161.25</v>
+      </c>
+      <c r="D438" t="n">
+        <v>110818.17</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>2025-09-07</t>
+        </is>
+      </c>
+      <c r="B439" t="n">
+        <v>111187.39</v>
+      </c>
+      <c r="C439" t="n">
+        <v>111176.54</v>
+      </c>
+      <c r="D439" t="n">
+        <v>110663.53</v>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>2025-09-08</t>
+        </is>
+      </c>
+      <c r="B440" t="n">
+        <v>112358.95</v>
+      </c>
+      <c r="C440" t="n">
+        <v>112204.42</v>
+      </c>
+      <c r="D440" t="n">
+        <v>111332.32</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="B441" t="n">
+        <v>112026.12</v>
+      </c>
+      <c r="C441" t="n">
+        <v>111292.34</v>
+      </c>
+      <c r="D441" t="n">
+        <v>113093.82</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="B442" t="n">
+        <v>114101.92</v>
+      </c>
+      <c r="C442" t="n">
+        <v>113415.66</v>
+      </c>
+      <c r="D442" t="n">
+        <v>112113.55</v>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="B443" t="n">
+        <v>114356.29</v>
+      </c>
+      <c r="C443" t="n">
+        <v>114386.02</v>
+      </c>
+      <c r="D443" t="n">
+        <v>114124.21</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>2025-09-12</t>
+        </is>
+      </c>
+      <c r="B444" t="n">
+        <v>115229.77</v>
+      </c>
+      <c r="C444" t="n">
+        <v>116586.5</v>
+      </c>
+      <c r="D444" t="n">
+        <v>115275.13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>